<commit_message>
Ensured initial MPS is right-normalized
</commit_message>
<xml_diff>
--- a/heisPractice/Worklist.xlsx
+++ b/heisPractice/Worklist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="460" windowWidth="24400" windowHeight="16480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1560" yWindow="460" windowWidth="24400" windowHeight="16340" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Array Sizes" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="43">
   <si>
     <t>nsite</t>
   </si>
@@ -151,6 +151,12 @@
   </si>
   <si>
     <t>My Hopt is not reshaping H the same as the other</t>
+  </si>
+  <si>
+    <t>We must exchange H indices in optimization H_opt</t>
+  </si>
+  <si>
+    <t>Write Function Explanations</t>
   </si>
 </sst>
 </file>
@@ -3134,7 +3140,7 @@
   <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3264,6 +3270,9 @@
       <c r="H4" t="s">
         <v>33</v>
       </c>
+      <c r="J4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C5">
@@ -3285,6 +3294,9 @@
       <c r="C7">
         <v>193</v>
       </c>
+      <c r="H7" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -3296,9 +3308,6 @@
       <c r="C8">
         <v>201</v>
       </c>
-      <c r="H8" s="28" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -3310,8 +3319,8 @@
       <c r="C9">
         <v>202</v>
       </c>
-      <c r="H9" t="s">
-        <v>36</v>
+      <c r="H9" s="28" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
@@ -3319,7 +3328,7 @@
         <v>206</v>
       </c>
       <c r="H10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
@@ -3327,12 +3336,15 @@
         <v>208</v>
       </c>
       <c r="H11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C12">
         <v>209</v>
+      </c>
+      <c r="H12" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">

</xml_diff>